<commit_message>
finished AD and all other model, ready to revise
</commit_message>
<xml_diff>
--- a/results/modelling_results.xlsx
+++ b/results/modelling_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t xml:space="preserve">validation Y</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t xml:space="preserve">MRE_all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validation prediction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing prediction</t>
   </si>
 </sst>
 </file>
@@ -148,16 +154,15 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D41:D42 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,17 +407,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D41:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.984693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,13 +427,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>4</v>
@@ -442,89 +449,197 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>75.3343091929</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>85.4673767089844</v>
+      </c>
       <c r="C2" s="0" t="n">
-        <v>110.17</v>
+        <v>110.17365474153</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>111.5</v>
+        <v>99.5393142700195</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>36.4</v>
+        <v>39.86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>38.1188930719</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>59.1052856445313</v>
+      </c>
       <c r="C3" s="0" t="n">
-        <v>52.26</v>
+        <v>52.258299428173</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>29.67</v>
+        <v>30.3464260101318</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>99.9226218037</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>86.4268112182617</v>
+      </c>
       <c r="C4" s="0" t="n">
-        <v>91.71</v>
+        <v>91.71323266061</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>34.37</v>
+        <v>47.0205917358399</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>73.3913166371</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>55.6705207824707</v>
+      </c>
       <c r="C5" s="0" t="n">
-        <v>232.88</v>
+        <v>232.88550969278</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>139.26</v>
+        <v>131.240203857422</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>86.6489246683</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>82.2365036010742</v>
+      </c>
       <c r="C6" s="0" t="n">
-        <v>288.14</v>
+        <v>288.14541835177</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>180.78</v>
+        <v>180.660690307617</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>97.6407610572</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>85.548942565918</v>
+      </c>
       <c r="C7" s="0" t="n">
-        <v>73.47</v>
+        <v>73.479614466793</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>98.41</v>
+        <v>101.070121765137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>101.3874286238</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>71.151237487793</v>
+      </c>
       <c r="C8" s="0" t="n">
-        <v>96.36</v>
+        <v>96.36471013916</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>131.82</v>
+        <v>151.055953979492</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>111.9314793025</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>54.3901138305664</v>
+      </c>
       <c r="C9" s="0" t="n">
-        <v>50.59</v>
+        <v>50.591904210414</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>86.2</v>
+        <v>89.4068069458008</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>87.6180861663</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>63.2286949157715</v>
+      </c>
       <c r="C10" s="0" t="n">
-        <v>83.76</v>
+        <v>83.76170589193</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>104.79</v>
+        <v>118.966529846191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>139.8541034812</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>111.470520019531</v>
+      </c>
       <c r="C11" s="0" t="n">
-        <v>76.72</v>
+        <v>76.722590928303</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>66.48</v>
+        <v>59.7607841491699</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>19.9327807577</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>53.6841278076172</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>22.7321777434</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>56.8656845092773</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>50.0834627166</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>49.0335197448731</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>195.8674698347</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>129.831283569336</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>66.1856214908</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>82.0281448364258</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>87.3141084414</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>82.417610168457</v>
       </c>
     </row>
   </sheetData>
@@ -546,12 +661,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D41:D42 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -572,12 +687,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D41:D42 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -598,12 +713,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D41:D42 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -624,12 +739,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D41:D42 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>